<commit_message>
Requerimientos Funcionales y no Funcionales
Cambio a un requerimiento funcional en su estado actual
</commit_message>
<xml_diff>
--- a/DSY1104 Evaluación Parcial 1 - Anexo 2 Planilla de Requerimientos.xlsx
+++ b/DSY1104 Evaluación Parcial 1 - Anexo 2 Planilla de Requerimientos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\papit\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Duoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7584DC9-E348-4F9B-AEA0-0B4E40748D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E8DB8B-BD29-4385-8DBE-923A7268064B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="1065" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instrucciones" sheetId="4" r:id="rId1"/>
@@ -724,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,7 +821,7 @@
         <v>43</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1024,15 +1024,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="e1e7bc46-bed0-459f-9452-a76b1c5b695e">
@@ -1040,6 +1031,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1254,19 +1254,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{370A914A-1DD7-4F78-8671-F61C286C2CC1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14168F1D-C031-4047-A789-A93363341739}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e1e7bc46-bed0-459f-9452-a76b1c5b695e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14168F1D-C031-4047-A789-A93363341739}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{370A914A-1DD7-4F78-8671-F61C286C2CC1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e1e7bc46-bed0-459f-9452-a76b1c5b695e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>